<commit_message>
EPBDS-9746 excel generation refactoring
--HG--
branch : EPBDS-9746
</commit_message>
<xml_diff>
--- a/Util/openl-excel-builder/resources/template.xlsx
+++ b/Util/openl-excel-builder/resources/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rom16\OneDrive\Документы\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Util\openl-excel-builder\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B586121B-C036-4441-A418-034B5BE23EDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31930D1D-2F29-4F40-A9ED-00419FDFC70B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15225" activeTab="1" xr2:uid="{ADD8EA8A-53B8-43DF-B81B-2EEF8E7885CB}"/>
+    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15225" xr2:uid="{ADD8EA8A-53B8-43DF-B81B-2EEF8E7885CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <r>
       <t xml:space="preserve">Datatype </t>
@@ -268,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -296,13 +296,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -342,6 +351,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -659,17 +674,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17A8EB3-D30F-4D48-9623-BC1DC34F036B}">
-  <dimension ref="B3:D4"/>
+  <dimension ref="B3:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="18.3125" customWidth="1"/>
     <col min="3" max="3" width="15.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
@@ -687,6 +702,17 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -703,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E38990-0B0F-4D5D-AC49-00E476A63352}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
EPBDS-10247	Enviroment table generation
</commit_message>
<xml_diff>
--- a/Util/openl-excel-builder/resources/template.xlsx
+++ b/Util/openl-excel-builder/resources/template.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Util\openl-excel-builder\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31930D1D-2F29-4F40-A9ED-00419FDFC70B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04107693-057B-4C2A-B1E2-A6698F256C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15225" xr2:uid="{ADD8EA8A-53B8-43DF-B81B-2EEF8E7885CB}"/>
+    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ADD8EA8A-53B8-43DF-B81B-2EEF8E7885CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
     <sheet name="SpreadsheetResults" sheetId="2" r:id="rId2"/>
     <sheet name="Vocabulary" sheetId="3" r:id="rId3"/>
+    <sheet name="Environment" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <r>
       <t xml:space="preserve">Datatype </t>
@@ -169,13 +170,25 @@
   </si>
   <si>
     <t>{spr.field.value}</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>regularRow</t>
+  </si>
+  <si>
+    <t>lastRow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +245,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -311,7 +330,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -346,17 +365,20 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -676,7 +698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17A8EB3-D30F-4D48-9623-BC1DC34F036B}">
   <dimension ref="B3:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -688,11 +710,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="1" t="s">
@@ -706,13 +728,13 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
     </row>
@@ -740,10 +762,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="6" t="s">
@@ -809,4 +831,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C443521-3CE6-4204-B5DC-D677EC79D4C7}">
+  <dimension ref="B3:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-10211 EPBDS-10214 EPBDS-9746 Remove needless hidden information, Use US localization.
</commit_message>
<xml_diff>
--- a/Util/openl-excel-builder/resources/template.xlsx
+++ b/Util/openl-excel-builder/resources/template.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Util\openl-excel-builder\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04107693-057B-4C2A-B1E2-A6698F256C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F00BE8-46BD-4F03-A8CC-1C107C8DC2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ADD8EA8A-53B8-43DF-B81B-2EEF8E7885CB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ADD8EA8A-53B8-43DF-B81B-2EEF8E7885CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
@@ -382,9 +377,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10 10" xfId="2" xr:uid="{5502B332-A237-49F7-A8A1-C6261C603972}"/>
     <cellStyle name="Normal 3 2 2 8" xfId="1" xr:uid="{940725CD-5DB4-4281-9B59-6DC40EAE982D}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,9 +395,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -440,7 +435,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -546,7 +541,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -702,21 +697,21 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.3125" customWidth="1"/>
-    <col min="3" max="3" width="15.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.578125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -727,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -755,19 +750,19 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.20703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="15"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
@@ -775,7 +770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
@@ -783,7 +778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
@@ -796,6 +791,7 @@
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -807,29 +803,30 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.3125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -841,15 +838,15 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
@@ -857,7 +854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
@@ -870,5 +867,6 @@
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-10250 generating data tables
</commit_message>
<xml_diff>
--- a/Util/openl-excel-builder/resources/template.xlsx
+++ b/Util/openl-excel-builder/resources/template.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F00BE8-46BD-4F03-A8CC-1C107C8DC2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C477A84E-9FF5-47CE-A495-08869E934CBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ADD8EA8A-53B8-43DF-B81B-2EEF8E7885CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{ADD8EA8A-53B8-43DF-B81B-2EEF8E7885CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
     <sheet name="SpreadsheetResults" sheetId="2" r:id="rId2"/>
     <sheet name="Vocabulary" sheetId="3" r:id="rId3"/>
     <sheet name="Environment" sheetId="4" r:id="rId4"/>
+    <sheet name="Data Table" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <r>
       <t xml:space="preserve">Datatype </t>
@@ -177,6 +178,69 @@
   </si>
   <si>
     <t>lastRow</t>
+  </si>
+  <si>
+    <t>Mileage</t>
+  </si>
+  <si>
+    <t>Vehicle Value</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>Fuel Type</t>
+  </si>
+  <si>
+    <t>Vehicle Body Type</t>
+  </si>
+  <si>
+    <t>Has AntiLock Brake</t>
+  </si>
+  <si>
+    <t>Coverages</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>Sport Van</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Coverage1, Coverage2, Coverage4</t>
+  </si>
+  <si>
+    <t>Model Year</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data {returnType} </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>{table.name}</t>
+    </r>
+  </si>
+  <si>
+    <t>{header.name}</t>
+  </si>
+  <si>
+    <t>{row.value}</t>
+  </si>
+  <si>
+    <t>{subheader.row}</t>
   </si>
 </sst>
 </file>
@@ -325,7 +389,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -366,6 +430,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,6 +451,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -705,11 +785,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -738,7 +818,7 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -757,10 +837,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -791,7 +871,7 @@
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -826,7 +906,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -834,17 +914,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C443521-3CE6-4204-B5DC-D677EC79D4C7}">
   <dimension ref="B3:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -867,6 +947,119 @@
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD72951-9E81-41D1-86E5-F36C44A266BA}">
+  <dimension ref="B3:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+    </row>
+    <row r="4" spans="2:10" ht="27" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="2:10" ht="27" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2012</v>
+      </c>
+      <c r="D6" s="16">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="16">
+        <v>9000</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>